<commit_message>
TAK update, Psychiatry addition
</commit_message>
<xml_diff>
--- a/ABBV.xlsx
+++ b/ABBV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF57C3DA-AEEC-42DE-8192-1CA0E8BB5E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44960056-7ABC-43A4-802D-E8018BF3951C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26115" yWindow="765" windowWidth="25470" windowHeight="20325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32850" yWindow="780" windowWidth="33270" windowHeight="20880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="4" r:id="rId1"/>
@@ -1120,13 +1120,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1346,167 +1352,169 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -1584,15 +1592,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>86915</xdr:colOff>
+      <xdr:colOff>27384</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>35718</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>86915</xdr:colOff>
+      <xdr:colOff>27384</xdr:colOff>
       <xdr:row>115</xdr:row>
-      <xdr:rowOff>54768</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1607,8 +1615,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="39371587" y="35718"/>
-          <a:ext cx="0" cy="18211800"/>
+          <a:off x="39312056" y="23812"/>
+          <a:ext cx="0" cy="18533269"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2243,8 +2251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2419,7 +2427,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="79" t="s">
         <v>168</v>
       </c>
       <c r="C7" s="36" t="s">
@@ -2508,7 +2516,7 @@
       <c r="H10" s="11"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="79" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="59" t="s">
@@ -3020,11 +3028,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:GQ111"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AQ3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AR6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AV6" sqref="AV6"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4428,7 +4436,7 @@
       </c>
     </row>
     <row r="11" spans="1:72" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="78" t="s">
         <v>121</v>
       </c>
       <c r="C11" s="16"/>
@@ -5179,7 +5187,7 @@
         <v>364</v>
       </c>
       <c r="AV15" s="16">
-        <f t="shared" ref="AU15:AX15" si="27">+AR15*0.9</f>
+        <f t="shared" ref="AV15:AX15" si="27">+AR15*0.9</f>
         <v>358.2</v>
       </c>
       <c r="AW15" s="16">
@@ -5517,7 +5525,7 @@
         <v>305</v>
       </c>
       <c r="AV17" s="16">
-        <f t="shared" ref="AU17:AX17" si="31">+AR17</f>
+        <f t="shared" ref="AV17:AX17" si="31">+AR17</f>
         <v>318</v>
       </c>
       <c r="AW17" s="16">
@@ -5682,7 +5690,7 @@
         <v>200</v>
       </c>
       <c r="AV18" s="16">
-        <f t="shared" ref="AU18:AX18" si="33">+AR18*0.95</f>
+        <f t="shared" ref="AV18:AX18" si="33">+AR18*0.95</f>
         <v>310.64999999999998</v>
       </c>
       <c r="AW18" s="16">
@@ -5847,7 +5855,7 @@
         <v>92</v>
       </c>
       <c r="AV19" s="16">
-        <f t="shared" ref="AU19:AX19" si="35">+AU19-10</f>
+        <f t="shared" ref="AV19:AX19" si="35">+AU19-10</f>
         <v>82</v>
       </c>
       <c r="AW19" s="16">
@@ -6012,7 +6020,7 @@
         <v>259</v>
       </c>
       <c r="AV20" s="16">
-        <f t="shared" ref="AU20:AX21" si="37">+AR20*0.95</f>
+        <f t="shared" ref="AV20:AX21" si="37">+AR20*0.95</f>
         <v>242.25</v>
       </c>
       <c r="AW20" s="16">
@@ -6342,7 +6350,7 @@
         <v>130</v>
       </c>
       <c r="AV22" s="16">
-        <f t="shared" ref="AU22:AX22" si="40">+AR22</f>
+        <f t="shared" ref="AV22:AX22" si="40">+AR22</f>
         <v>130</v>
       </c>
       <c r="AW22" s="16">
@@ -6845,7 +6853,7 @@
         <v>71</v>
       </c>
       <c r="AV25" s="16">
-        <f t="shared" ref="AU25:AX25" si="45">+AU25-3</f>
+        <f t="shared" ref="AV25:AX25" si="45">+AU25-3</f>
         <v>68</v>
       </c>
       <c r="AW25" s="16">
@@ -8854,7 +8862,7 @@
         <v>691</v>
       </c>
       <c r="AV42" s="16">
-        <f t="shared" ref="AU42:AX42" si="48">+AR42*0.9</f>
+        <f t="shared" ref="AV42:AX42" si="48">+AR42*0.9</f>
         <v>908.1</v>
       </c>
       <c r="AW42" s="16">
@@ -10769,7 +10777,7 @@
         <v>781</v>
       </c>
       <c r="AV52" s="16">
-        <f t="shared" ref="AU52:AX52" si="115">+AV51*0.15</f>
+        <f t="shared" ref="AV52:AX52" si="115">+AV51*0.15</f>
         <v>1199.289</v>
       </c>
       <c r="AW52" s="16">
@@ -11871,7 +11879,7 @@
         <v>1776</v>
       </c>
       <c r="AV55" s="16">
-        <f t="shared" ref="AU55:AX55" si="146">+AU55</f>
+        <f t="shared" ref="AV55:AX55" si="146">+AU55</f>
         <v>1776</v>
       </c>
       <c r="AW55" s="16">
@@ -12487,55 +12495,55 @@
         <v>8.9896579156722334E-2</v>
       </c>
       <c r="AL60" s="30">
-        <f>+AL7/AH7-1</f>
+        <f t="shared" ref="AL60:AX61" si="167">+AL7/AH7-1</f>
         <v>9.8765432098765427E-2</v>
       </c>
       <c r="AM60" s="30">
-        <f>+AM7/AI7-1</f>
+        <f t="shared" si="167"/>
         <v>2.9220779220779258E-2</v>
       </c>
       <c r="AN60" s="30">
-        <f>+AN7/AJ7-1</f>
+        <f t="shared" si="167"/>
         <v>7.2204968944099335E-2</v>
       </c>
       <c r="AO60" s="30">
-        <f>+AO7/AK7-1</f>
+        <f t="shared" si="167"/>
         <v>2.9197080291971655E-3</v>
       </c>
       <c r="AP60" s="30">
-        <f>+AP7/AL7-1</f>
+        <f t="shared" si="167"/>
         <v>-2.73876404494382E-2</v>
       </c>
       <c r="AQ60" s="30">
-        <f>+AQ7/AM7-1</f>
+        <f t="shared" si="167"/>
         <v>-7.4921135646687675E-2</v>
       </c>
       <c r="AR60" s="30">
-        <f>+AR7/AN7-1</f>
+        <f t="shared" si="167"/>
         <v>-0.17089065894279509</v>
       </c>
       <c r="AS60" s="30">
-        <f>+AS7/AO7-1</f>
+        <f t="shared" si="167"/>
         <v>-0.17394468704512378</v>
       </c>
       <c r="AT60" s="30">
-        <f>+AT7/AP7-1</f>
+        <f t="shared" si="167"/>
         <v>-0.19494584837545126</v>
       </c>
       <c r="AU60" s="30">
-        <f>+AU7/AQ7-1</f>
+        <f t="shared" si="167"/>
         <v>-0.25149190110826936</v>
       </c>
       <c r="AV60" s="30">
-        <f>+AV7/AR7-1</f>
+        <f t="shared" si="167"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="AW60" s="30">
-        <f>+AW7/AS7-1</f>
+        <f t="shared" si="167"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="AX60" s="30">
-        <f>+AX7/AT7-1</f>
+        <f t="shared" si="167"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="AY60" s="30"/>
@@ -12557,43 +12565,43 @@
         <v>0.13692768506632436</v>
       </c>
       <c r="BK60" s="30">
-        <f t="shared" ref="BK60:BT60" si="167">+BK7/BJ7-1</f>
+        <f t="shared" ref="BK60:BT60" si="168">+BK7/BJ7-1</f>
         <v>1.7689123071132906E-2</v>
       </c>
       <c r="BL60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-0.15532544378698221</v>
       </c>
       <c r="BM60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-0.10000000000000009</v>
       </c>
       <c r="BN60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BO60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BP60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BQ60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BR60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BS60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-0.10000000000000009</v>
       </c>
       <c r="BT60" s="30">
-        <f t="shared" si="167"/>
+        <f t="shared" si="168"/>
         <v>-9.9999999999999978E-2</v>
       </c>
       <c r="BV60" s="51" t="s">
@@ -12668,63 +12676,63 @@
         <v>212</v>
       </c>
       <c r="AJ61" s="30">
-        <f t="shared" ref="AJ61:AK61" si="168">+AJ8/AF8-1</f>
+        <f t="shared" ref="AJ61:AK61" si="169">+AJ8/AF8-1</f>
         <v>5.875</v>
       </c>
       <c r="AK61" s="30">
-        <f t="shared" si="168"/>
+        <f t="shared" si="169"/>
         <v>3.7802197802197801</v>
       </c>
       <c r="AL61" s="30">
-        <f>+AL8/AH8-1</f>
+        <f t="shared" si="167"/>
         <v>1.4305555555555554</v>
       </c>
       <c r="AM61" s="30">
-        <f>+AM8/AI8-1</f>
+        <f t="shared" si="167"/>
         <v>0.91333333333333333</v>
       </c>
       <c r="AN61" s="30">
-        <f>+AN8/AJ8-1</f>
+        <f t="shared" si="167"/>
         <v>1.0424242424242425</v>
       </c>
       <c r="AO61" s="30">
-        <f>+AO8/AK8-1</f>
+        <f t="shared" si="167"/>
         <v>0.8298850574712644</v>
       </c>
       <c r="AP61" s="30">
-        <f>+AP8/AL8-1</f>
+        <f t="shared" si="167"/>
         <v>0.7047619047619047</v>
       </c>
       <c r="AQ61" s="30">
-        <f>+AQ8/AM8-1</f>
+        <f t="shared" si="167"/>
         <v>0.63763066202090601</v>
       </c>
       <c r="AR61" s="30">
-        <f>+AR8/AN8-1</f>
+        <f t="shared" si="167"/>
         <v>0.85756676557863498</v>
       </c>
       <c r="AS61" s="30">
-        <f>+AS8/AO8-1</f>
+        <f t="shared" si="167"/>
         <v>0.75502512562814061</v>
       </c>
       <c r="AT61" s="30">
-        <f>+AT8/AP8-1</f>
+        <f t="shared" si="167"/>
         <v>0.76089385474860327</v>
       </c>
       <c r="AU61" s="30">
-        <f>+AU8/AQ8-1</f>
+        <f t="shared" si="167"/>
         <v>0.44680851063829796</v>
       </c>
       <c r="AV61" s="30">
-        <f>+AV8/AR8-1</f>
+        <f t="shared" si="167"/>
         <v>0.5</v>
       </c>
       <c r="AW61" s="30">
-        <f>+AW8/AS8-1</f>
+        <f t="shared" si="167"/>
         <v>0.39999999999999991</v>
       </c>
       <c r="AX61" s="30">
-        <f>+AX8/AT8-1</f>
+        <f t="shared" si="167"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="AY61" s="30"/>
@@ -12745,43 +12753,43 @@
         <v>3.47887323943662</v>
       </c>
       <c r="BK61" s="30">
-        <f t="shared" ref="BK61:BT61" si="169">+BK8/BJ8-1</f>
+        <f t="shared" ref="BK61:BT61" si="170">+BK8/BJ8-1</f>
         <v>0.84842767295597477</v>
       </c>
       <c r="BL61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>0.75740047635250085</v>
       </c>
       <c r="BM61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="BN61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="BO61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="BP61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="BQ61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="BR61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="BS61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="BT61" s="30">
-        <f t="shared" si="169"/>
+        <f t="shared" si="170"/>
         <v>3.0000000000000027E-2</v>
       </c>
     </row>
@@ -12818,7 +12826,7 @@
       <c r="AC62" s="30"/>
       <c r="AD62" s="30"/>
       <c r="AE62" s="30">
-        <f t="shared" ref="AE62" si="170">+AE3/AA3-1</f>
+        <f t="shared" ref="AE62" si="171">+AE3/AA3-1</f>
         <v>-5.5850499044383106E-2</v>
       </c>
       <c r="AF62" s="30">
@@ -12826,75 +12834,75 @@
         <v>-5.1494696239151372E-2</v>
       </c>
       <c r="AG62" s="30">
-        <f t="shared" ref="AG62:AL62" si="171">+AG3/AC3-1</f>
+        <f t="shared" ref="AG62:AL62" si="172">+AG3/AC3-1</f>
         <v>-1.6198282591725177E-2</v>
       </c>
       <c r="AH62" s="30">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>5.0427002846685554E-2</v>
       </c>
       <c r="AI62" s="30">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>0.14462438146648671</v>
       </c>
       <c r="AJ62" s="30">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>8.0927206181374611E-2</v>
       </c>
       <c r="AK62" s="30">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>0.14858163062884344</v>
       </c>
       <c r="AL62" s="30">
-        <f t="shared" si="171"/>
+        <f t="shared" si="172"/>
         <v>0.1533101045296168</v>
       </c>
       <c r="AM62" s="30">
-        <f t="shared" ref="AM62" si="172">+AM3/AI3-1</f>
+        <f t="shared" ref="AM62" si="173">+AM3/AI3-1</f>
         <v>0.1287089801532717</v>
       </c>
       <c r="AN62" s="30">
-        <f t="shared" ref="AN62" si="173">+AN3/AJ3-1</f>
+        <f t="shared" ref="AN62" si="174">+AN3/AJ3-1</f>
         <v>0.15124153498871329</v>
       </c>
       <c r="AO62" s="30">
-        <f t="shared" ref="AO62" si="174">+AO3/AK3-1</f>
+        <f t="shared" ref="AO62" si="175">+AO3/AK3-1</f>
         <v>0.15267702936096716</v>
       </c>
       <c r="AP62" s="30">
-        <f t="shared" ref="AP62" si="175">+AP3/AL3-1</f>
+        <f t="shared" ref="AP62" si="176">+AP3/AL3-1</f>
         <v>0.13225914736488753</v>
       </c>
       <c r="AQ62" s="30">
-        <f t="shared" ref="AQ62" si="176">+AQ3/AM3-1</f>
+        <f t="shared" ref="AQ62" si="177">+AQ3/AM3-1</f>
         <v>6.9115598885793883E-2</v>
       </c>
       <c r="AR62" s="30">
-        <f t="shared" ref="AR62" si="177">+AR3/AN3-1</f>
+        <f t="shared" ref="AR62" si="178">+AR3/AN3-1</f>
         <v>0.17761437908496736</v>
       </c>
       <c r="AS62" s="30">
-        <f t="shared" ref="AS62" si="178">+AS3/AO3-1</f>
+        <f t="shared" ref="AS62" si="179">+AS3/AO3-1</f>
         <v>0.14638897213065638</v>
       </c>
       <c r="AT62" s="30">
-        <f t="shared" ref="AT62" si="179">+AT3/AP3-1</f>
+        <f t="shared" ref="AT62" si="180">+AT3/AP3-1</f>
         <v>0.17477023421286697</v>
       </c>
       <c r="AU62" s="30">
-        <f t="shared" ref="AU62" si="180">+AU3/AQ3-1</f>
+        <f t="shared" ref="AU62" si="181">+AU3/AQ3-1</f>
         <v>-9.0213320306139044E-2</v>
       </c>
       <c r="AV62" s="30">
-        <f t="shared" ref="AV62" si="181">+AV3/AR3-1</f>
+        <f t="shared" ref="AV62" si="182">+AV3/AR3-1</f>
         <v>-0.19436658803940632</v>
       </c>
       <c r="AW62" s="30">
-        <f t="shared" ref="AW62" si="182">+AW3/AS3-1</f>
+        <f t="shared" ref="AW62" si="183">+AW3/AS3-1</f>
         <v>-0.27208208077375506</v>
       </c>
       <c r="AX62" s="30">
-        <f t="shared" ref="AX62" si="183">+AX3/AT3-1</f>
+        <f t="shared" ref="AX62" si="184">+AX3/AT3-1</f>
         <v>-0.34329337539432181</v>
       </c>
       <c r="AY62" s="30"/>
@@ -13032,47 +13040,47 @@
         <v>212</v>
       </c>
       <c r="AN63" s="30">
-        <f>AN9/AJ9-1</f>
+        <f t="shared" ref="AN63:AX64" si="185">AN9/AJ9-1</f>
         <v>1.584070796460177</v>
       </c>
       <c r="AO63" s="30">
-        <f>AO9/AK9-1</f>
+        <f t="shared" si="185"/>
         <v>0.38676844783715003</v>
       </c>
       <c r="AP63" s="30">
-        <f>AP9/AL9-1</f>
+        <f t="shared" si="185"/>
         <v>0.26977687626774838</v>
       </c>
       <c r="AQ63" s="30">
-        <f>AQ9/AM9-1</f>
+        <f t="shared" si="185"/>
         <v>0.34381551362683438</v>
       </c>
       <c r="AR63" s="30">
-        <f>AR9/AN9-1</f>
+        <f t="shared" si="185"/>
         <v>0.19006849315068486</v>
       </c>
       <c r="AS63" s="30">
-        <f>AS9/AO9-1</f>
+        <f t="shared" si="185"/>
         <v>0.16880733944954129</v>
       </c>
       <c r="AT63" s="30">
-        <f>AT9/AP9-1</f>
+        <f t="shared" si="185"/>
         <v>2.5559105431310014E-2</v>
       </c>
       <c r="AU63" s="30">
-        <f>AU9/AQ9-1</f>
+        <f t="shared" si="185"/>
         <v>2.808112324492984E-2</v>
       </c>
       <c r="AV63" s="30">
-        <f>AV9/AR9-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AW63" s="30">
-        <f>AW9/AS9-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AX63" s="30">
-        <f>AX9/AT9-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AY63" s="30"/>
@@ -13173,47 +13181,47 @@
         <v>212</v>
       </c>
       <c r="AN64" s="30">
-        <f>AN10/AJ10-1</f>
+        <f t="shared" si="185"/>
         <v>1.0303030303030303</v>
       </c>
       <c r="AO64" s="30">
-        <f>AO10/AK10-1</f>
+        <f t="shared" si="185"/>
         <v>0.23326959847036322</v>
       </c>
       <c r="AP64" s="30">
-        <f>AP10/AL10-1</f>
+        <f t="shared" si="185"/>
         <v>0.18342151675485008</v>
       </c>
       <c r="AQ64" s="30">
-        <f>AQ10/AM10-1</f>
+        <f t="shared" si="185"/>
         <v>0.15413533834586457</v>
       </c>
       <c r="AR64" s="30">
-        <f>AR10/AN10-1</f>
+        <f t="shared" si="185"/>
         <v>0.12437810945273631</v>
       </c>
       <c r="AS64" s="30">
-        <f>AS10/AO10-1</f>
+        <f t="shared" si="185"/>
         <v>8.3720930232558111E-2</v>
       </c>
       <c r="AT64" s="30">
-        <f>AT10/AP10-1</f>
+        <f t="shared" si="185"/>
         <v>8.4947839046199736E-2</v>
       </c>
       <c r="AU64" s="30">
-        <f>AU10/AQ10-1</f>
+        <f t="shared" si="185"/>
         <v>0.17100977198697076</v>
       </c>
       <c r="AV64" s="30">
-        <f>AV10/AR10-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AW64" s="30">
-        <f>AW10/AS10-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AX64" s="30">
-        <f>AX10/AT10-1</f>
+        <f t="shared" si="185"/>
         <v>3.0000000000000027E-2</v>
       </c>
       <c r="AY64" s="30"/>
@@ -13305,35 +13313,35 @@
         <v>212</v>
       </c>
       <c r="AK65" s="30">
-        <f t="shared" ref="AK65:AT65" si="184">AK12/AG12-1</f>
+        <f t="shared" ref="AK65:AT65" si="186">AK12/AG12-1</f>
         <v>14.357142857142858</v>
       </c>
       <c r="AL65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>7.5151515151515156</v>
       </c>
       <c r="AM65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>2.5232558139534884</v>
       </c>
       <c r="AN65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>1.5369127516778525</v>
       </c>
       <c r="AO65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>1.1069767441860465</v>
       </c>
       <c r="AP65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>0.83985765124555156</v>
       </c>
       <c r="AQ65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>0.53465346534653468</v>
       </c>
       <c r="AR65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>0.56613756613756605</v>
       </c>
       <c r="AS65" s="30">
@@ -13341,23 +13349,23 @@
         <v>0.53421633554083892</v>
       </c>
       <c r="AT65" s="30">
-        <f t="shared" si="184"/>
+        <f t="shared" si="186"/>
         <v>0.4893617021276595</v>
       </c>
       <c r="AU65" s="30">
-        <f t="shared" ref="AU65" si="185">AU12/AQ12-1</f>
+        <f t="shared" ref="AU65" si="187">AU12/AQ12-1</f>
         <v>0.47526881720430114</v>
       </c>
       <c r="AV65" s="30">
-        <f t="shared" ref="AV65" si="186">AV12/AR12-1</f>
+        <f t="shared" ref="AV65" si="188">AV12/AR12-1</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="AW65" s="30">
-        <f t="shared" ref="AW65" si="187">AW12/AS12-1</f>
+        <f t="shared" ref="AW65" si="189">AW12/AS12-1</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="AX65" s="30">
-        <f t="shared" ref="AX65" si="188">AX12/AT12-1</f>
+        <f t="shared" ref="AX65" si="190">AX12/AT12-1</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="AY65" s="30"/>
@@ -13481,39 +13489,39 @@
       <c r="W67" s="30"/>
       <c r="X67" s="30"/>
       <c r="Y67" s="30">
-        <f t="shared" ref="Y67" si="189">+Y45/Y43</f>
+        <f t="shared" ref="Y67" si="191">+Y45/Y43</f>
         <v>0.80814867762687637</v>
       </c>
       <c r="Z67" s="30">
-        <f t="shared" ref="Z67" si="190">+Z45/Z43</f>
+        <f t="shared" ref="Z67" si="192">+Z45/Z43</f>
         <v>0.78989533531464018</v>
       </c>
       <c r="AA67" s="30">
-        <f t="shared" ref="AA67" si="191">+AA45/AA43</f>
+        <f t="shared" ref="AA67" si="193">+AA45/AA43</f>
         <v>0.80186538946307029</v>
       </c>
       <c r="AB67" s="30">
-        <f t="shared" ref="AB67:AG67" si="192">+AB45/AB43</f>
+        <f t="shared" ref="AB67:AG67" si="194">+AB45/AB43</f>
         <v>0.80540082344393316</v>
       </c>
       <c r="AC67" s="30">
-        <f t="shared" si="192"/>
+        <f t="shared" si="194"/>
         <v>0.81677999028654691</v>
       </c>
       <c r="AD67" s="30">
-        <f t="shared" si="192"/>
+        <f t="shared" si="194"/>
         <v>0.79843467790487654</v>
       </c>
       <c r="AE67" s="30">
-        <f t="shared" si="192"/>
+        <f t="shared" si="194"/>
         <v>0.83354624425140522</v>
       </c>
       <c r="AF67" s="30">
-        <f t="shared" si="192"/>
+        <f t="shared" si="194"/>
         <v>0.8271350696547547</v>
       </c>
       <c r="AG67" s="30">
-        <f t="shared" si="192"/>
+        <f t="shared" si="194"/>
         <v>0.82014388489208634</v>
       </c>
       <c r="AH67" s="30">
@@ -13533,31 +13541,31 @@
         <v>0.81664337835739786</v>
       </c>
       <c r="AL67" s="30">
-        <f t="shared" ref="AL67:AT67" si="193">+AL45/AL43</f>
+        <f t="shared" ref="AL67:AT67" si="195">+AL45/AL43</f>
         <v>0.81793909655072883</v>
       </c>
       <c r="AM67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.83880943177425593</v>
       </c>
       <c r="AN67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.82240848198295002</v>
       </c>
       <c r="AO67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.83175289359921911</v>
       </c>
       <c r="AP67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.83555018137847648</v>
       </c>
       <c r="AQ67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.84465947702762589</v>
       </c>
       <c r="AR67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.85140231776726327</v>
       </c>
       <c r="AS67" s="30">
@@ -13565,23 +13573,23 @@
         <v>0.85369970294355924</v>
       </c>
       <c r="AT67" s="30">
-        <f t="shared" si="193"/>
+        <f t="shared" si="195"/>
         <v>0.85</v>
       </c>
       <c r="AU67" s="30">
-        <f t="shared" ref="AU67:AX67" si="194">+AU45/AU43</f>
+        <f t="shared" ref="AU67:AX67" si="196">+AU45/AU43</f>
         <v>0.84204498977505116</v>
       </c>
       <c r="AV67" s="30">
-        <f t="shared" si="194"/>
+        <f t="shared" si="196"/>
         <v>0.85</v>
       </c>
       <c r="AW67" s="30">
-        <f t="shared" si="194"/>
+        <f t="shared" si="196"/>
         <v>0.85</v>
       </c>
       <c r="AX67" s="30">
-        <f t="shared" si="194"/>
+        <f t="shared" si="196"/>
         <v>0.85</v>
       </c>
       <c r="AY67" s="30"/>
@@ -13614,23 +13622,23 @@
         <v>0.85005081475867295</v>
       </c>
       <c r="BM67" s="30">
-        <f t="shared" ref="BM67:BQ67" si="195">+BM45/BM43</f>
+        <f t="shared" ref="BM67:BQ67" si="197">+BM45/BM43</f>
         <v>0.85</v>
       </c>
       <c r="BN67" s="30">
-        <f t="shared" si="195"/>
+        <f t="shared" si="197"/>
         <v>0.85</v>
       </c>
       <c r="BO67" s="30">
-        <f t="shared" si="195"/>
+        <f t="shared" si="197"/>
         <v>0.84999999999999987</v>
       </c>
       <c r="BP67" s="30">
-        <f t="shared" si="195"/>
+        <f t="shared" si="197"/>
         <v>0.85</v>
       </c>
       <c r="BQ67" s="30">
-        <f t="shared" si="195"/>
+        <f t="shared" si="197"/>
         <v>0.85</v>
       </c>
       <c r="BR67" s="30"/>
@@ -13663,39 +13671,39 @@
       <c r="W68" s="30"/>
       <c r="X68" s="30"/>
       <c r="Y68" s="30">
-        <f t="shared" ref="Y68" si="196">+Y52/Y51</f>
+        <f t="shared" ref="Y68" si="198">+Y52/Y51</f>
         <v>0.18934280639431617</v>
       </c>
       <c r="Z68" s="30">
-        <f t="shared" ref="Z68" si="197">+Z52/Z51</f>
+        <f t="shared" ref="Z68" si="199">+Z52/Z51</f>
         <v>0.18853848762292302</v>
       </c>
       <c r="AA68" s="30">
-        <f t="shared" ref="AA68" si="198">+AA52/AA51</f>
+        <f t="shared" ref="AA68" si="200">+AA52/AA51</f>
         <v>7.6450721522873813E-2</v>
       </c>
       <c r="AB68" s="30">
-        <f t="shared" ref="AB68:AG68" si="199">+AB52/AB51</f>
+        <f t="shared" ref="AB68:AG68" si="201">+AB52/AB51</f>
         <v>9.0040532715691957E-2</v>
       </c>
       <c r="AC68" s="30">
-        <f t="shared" si="199"/>
+        <f t="shared" si="201"/>
         <v>9.1036023457134879E-2</v>
       </c>
       <c r="AD68" s="30">
-        <f t="shared" si="199"/>
+        <f t="shared" si="201"/>
         <v>9.1716915264995244E-2</v>
       </c>
       <c r="AE68" s="30">
-        <f t="shared" si="199"/>
+        <f t="shared" si="201"/>
         <v>7.8917050691244245E-2</v>
       </c>
       <c r="AF68" s="30">
-        <f t="shared" si="199"/>
+        <f t="shared" si="201"/>
         <v>8.7567567567567561E-2</v>
       </c>
       <c r="AG68" s="30">
-        <f t="shared" si="199"/>
+        <f t="shared" si="201"/>
         <v>8.7848500789058384E-2</v>
       </c>
       <c r="AH68" s="30">
@@ -13715,31 +13723,31 @@
         <v>9.6755504055619931E-2</v>
       </c>
       <c r="AL68" s="30">
-        <f t="shared" ref="AL68:AT68" si="200">+AL52/AL51</f>
+        <f t="shared" ref="AL68:AT68" si="202">+AL52/AL51</f>
         <v>9.6443132292984679E-2</v>
       </c>
       <c r="AM68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.1234113712374582</v>
       </c>
       <c r="AN68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.12653834017040075</v>
       </c>
       <c r="AO68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.12783291364242336</v>
       </c>
       <c r="AP68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.12496302868973676</v>
       </c>
       <c r="AQ68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.11802184466019418</v>
       </c>
       <c r="AR68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.12982644961657475</v>
       </c>
       <c r="AS68" s="30">
@@ -13747,23 +13755,23 @@
         <v>0.1274432118330692</v>
       </c>
       <c r="AT68" s="30">
-        <f t="shared" si="200"/>
+        <f t="shared" si="202"/>
         <v>0.15</v>
       </c>
       <c r="AU68" s="30">
-        <f t="shared" ref="AU68:AX68" si="201">+AU52/AU51</f>
+        <f t="shared" ref="AU68:AX68" si="203">+AU52/AU51</f>
         <v>0.1364907375043691</v>
       </c>
       <c r="AV68" s="30">
-        <f t="shared" si="201"/>
+        <f t="shared" si="203"/>
         <v>0.15</v>
       </c>
       <c r="AW68" s="30">
-        <f t="shared" si="201"/>
+        <f t="shared" si="203"/>
         <v>0.15</v>
       </c>
       <c r="AX68" s="30">
-        <f t="shared" si="201"/>
+        <f t="shared" si="203"/>
         <v>0.15</v>
       </c>
       <c r="AY68" s="30"/>
@@ -13776,43 +13784,43 @@
       <c r="BF68" s="30"/>
       <c r="BG68" s="30"/>
       <c r="BH68" s="30">
-        <f t="shared" ref="BH68" si="202">+BH52/BH51</f>
+        <f t="shared" ref="BH68" si="204">+BH52/BH51</f>
         <v>8.7406084951275761E-2</v>
       </c>
       <c r="BI68" s="30">
-        <f t="shared" ref="BI68:BQ68" si="203">+BI52/BI51</f>
+        <f t="shared" ref="BI68:BQ68" si="205">+BI52/BI51</f>
         <v>8.5823964902659713E-2</v>
       </c>
       <c r="BJ68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.10015614543832255</v>
       </c>
       <c r="BK68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.12574038945453136</v>
       </c>
       <c r="BL68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.13161795219388039</v>
       </c>
       <c r="BM68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.15</v>
       </c>
       <c r="BN68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.15</v>
       </c>
       <c r="BO68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.15</v>
       </c>
       <c r="BP68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.15</v>
       </c>
       <c r="BQ68" s="30">
-        <f t="shared" si="203"/>
+        <f t="shared" si="205"/>
         <v>0.15</v>
       </c>
       <c r="BR68" s="30"/>

</xml_diff>